<commit_message>
Making new changes to the document and validations
</commit_message>
<xml_diff>
--- a/.dev/machine_registers.xlsx
+++ b/.dev/machine_registers.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>register_id</t>
   </si>
@@ -50,6 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -298,6 +301,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -318,17 +322,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="b">
+      <c r="C2" t="b" s="0">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>12974.0</v>
+      <c r="D2" t="n" s="0">
+        <v>5342.0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>